<commit_message>
List of bugs updated, few minor bugs fixed
</commit_message>
<xml_diff>
--- a/WinArc/Delphi_WinArc_BugReport.xlsx
+++ b/WinArc/Delphi_WinArc_BugReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Project</t>
   </si>
@@ -77,18 +77,35 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Creating zip-archive, that contains folder.</t>
+  </si>
+  <si>
+    <t>Folder icons in file system view are absent.</t>
+  </si>
+  <si>
+    <t>There isn't any constant local that contains number of columns for folder view.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,30 +170,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,13 +513,14 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="88.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -526,27 +547,27 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
@@ -554,13 +575,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
@@ -568,13 +589,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
@@ -582,13 +603,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
@@ -596,13 +617,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
@@ -610,13 +631,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
@@ -624,16 +645,52 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>